<commit_message>
test, ce lahko editam excel pa se ga da commitat
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejcjenko/Documents/FP/Projekt/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejcjenko/Documents/GitHub/Pareto-fronte-v-vec-dimenzijah/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{932A50F9-525E-B54D-942A-1683E491EE62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08223955-2D01-BB4A-9964-C072E3A8B818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="15680" xr2:uid="{70F57464-07EE-6D44-894E-A2427728D4C0}"/>
   </bookViews>
@@ -127,10 +127,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -447,8 +447,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1C919C-7229-7041-875E-3BE3CDC2D46A}">
   <dimension ref="B2:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J34" sqref="J34"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="G52" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -460,20 +460,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -556,7 +556,7 @@
         <v>4</v>
       </c>
       <c r="I8">
-        <f t="shared" ref="I8:I16" si="0">SUM(D8:H8)</f>
+        <f t="shared" ref="I8:I10" si="0">SUM(D8:H8)</f>
         <v>47</v>
       </c>
     </row>
@@ -637,7 +637,7 @@
         <v>4</v>
       </c>
       <c r="I11">
-        <f>SUM(D11:H11)</f>
+        <f t="shared" ref="I11:I16" si="1">SUM(D11:H11)</f>
         <v>48</v>
       </c>
     </row>
@@ -664,7 +664,7 @@
         <v>4</v>
       </c>
       <c r="I12">
-        <f>SUM(D12:H12)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
     </row>
@@ -691,7 +691,7 @@
         <v>2</v>
       </c>
       <c r="I13">
-        <f>SUM(D13:H13)</f>
+        <f t="shared" si="1"/>
         <v>46</v>
       </c>
     </row>
@@ -718,7 +718,7 @@
         <v>4</v>
       </c>
       <c r="I14">
-        <f>SUM(D14:H14)</f>
+        <f t="shared" si="1"/>
         <v>44</v>
       </c>
     </row>
@@ -745,7 +745,7 @@
         <v>3</v>
       </c>
       <c r="I15">
-        <f>SUM(D15:H15)</f>
+        <f t="shared" si="1"/>
         <v>42</v>
       </c>
     </row>
@@ -772,7 +772,7 @@
         <v>2</v>
       </c>
       <c r="I16">
-        <f>SUM(D16:H16)</f>
+        <f t="shared" si="1"/>
         <v>48</v>
       </c>
     </row>
@@ -781,27 +781,27 @@
         <v>7</v>
       </c>
       <c r="D17">
-        <f>AVERAGE(D7:D16)</f>
+        <f t="shared" ref="D17:I17" si="2">AVERAGE(D7:D16)</f>
         <v>11</v>
       </c>
       <c r="E17">
-        <f>AVERAGE(E7:E16)</f>
+        <f t="shared" si="2"/>
         <v>14.8</v>
       </c>
       <c r="F17">
-        <f>AVERAGE(F7:F16)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="G17">
-        <f>AVERAGE(G7:G16)</f>
+        <f t="shared" si="2"/>
         <v>6.2</v>
       </c>
       <c r="H17">
-        <f>AVERAGE(H7:H16)</f>
+        <f t="shared" si="2"/>
         <v>3.4</v>
       </c>
       <c r="I17">
-        <f>AVERAGE(I7:I16)</f>
+        <f t="shared" si="2"/>
         <v>46.4</v>
       </c>
     </row>
@@ -886,7 +886,7 @@
         <v>11</v>
       </c>
       <c r="I22">
-        <f t="shared" ref="I22:I31" si="1">SUM(D22:H22)</f>
+        <f t="shared" ref="I22:I31" si="3">SUM(D22:H22)</f>
         <v>88</v>
       </c>
     </row>
@@ -913,7 +913,7 @@
         <v>8</v>
       </c>
       <c r="I23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
     </row>
@@ -940,7 +940,7 @@
         <v>8</v>
       </c>
       <c r="I24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
     </row>
@@ -967,7 +967,7 @@
         <v>22</v>
       </c>
       <c r="I25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>83</v>
       </c>
     </row>
@@ -994,7 +994,7 @@
         <v>14</v>
       </c>
       <c r="I26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>79</v>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
         <v>15</v>
       </c>
       <c r="I27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
     </row>
@@ -1048,7 +1048,7 @@
         <v>8</v>
       </c>
       <c r="I28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>87</v>
       </c>
     </row>
@@ -1075,7 +1075,7 @@
         <v>12</v>
       </c>
       <c r="I29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
     </row>
@@ -1102,7 +1102,7 @@
         <v>6</v>
       </c>
       <c r="I30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>89</v>
       </c>
     </row>
@@ -1131,7 +1131,7 @@
         <v>11.4</v>
       </c>
       <c r="I31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>84.4</v>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
         <v>22</v>
       </c>
       <c r="I36">
-        <f t="shared" ref="I36:I44" si="2">SUM(D36:H36)</f>
+        <f t="shared" ref="I36:I44" si="4">SUM(D36:H36)</f>
         <v>117</v>
       </c>
     </row>
@@ -1243,7 +1243,7 @@
         <v>26</v>
       </c>
       <c r="I37">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>130</v>
       </c>
     </row>
@@ -1270,7 +1270,7 @@
         <v>32</v>
       </c>
       <c r="I38">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>146</v>
       </c>
     </row>
@@ -1297,7 +1297,7 @@
         <v>31</v>
       </c>
       <c r="I39">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>137</v>
       </c>
     </row>
@@ -1324,7 +1324,7 @@
         <v>23</v>
       </c>
       <c r="I40">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>126</v>
       </c>
     </row>
@@ -1351,7 +1351,7 @@
         <v>32</v>
       </c>
       <c r="I41">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>114</v>
       </c>
     </row>
@@ -1378,7 +1378,7 @@
         <v>35</v>
       </c>
       <c r="I42">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>165</v>
       </c>
     </row>
@@ -1405,7 +1405,7 @@
         <v>27</v>
       </c>
       <c r="I43">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>136</v>
       </c>
     </row>
@@ -1432,7 +1432,7 @@
         <v>24</v>
       </c>
       <c r="I44">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>133</v>
       </c>
     </row>
@@ -1461,7 +1461,7 @@
         <v>27.9</v>
       </c>
       <c r="I45">
-        <f t="shared" ref="I36:I45" si="3">SUM(D45:H45)</f>
+        <f t="shared" ref="I45" si="5">SUM(D45:H45)</f>
         <v>134.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
excel 2. del eksperimenta
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nejcjenko/Documents/GitHub/Pareto-fronte-v-vec-dimenzijah/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2AA999B-CB02-484F-8EFA-F9A27F4061A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EBEC2E8B-29C7-654A-9259-116CDFA198C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="15680" activeTab="4" xr2:uid="{70F57464-07EE-6D44-894E-A2427728D4C0}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="27640" windowHeight="15680" activeTab="5" xr2:uid="{70F57464-07EE-6D44-894E-A2427728D4C0}"/>
   </bookViews>
   <sheets>
     <sheet name="2 dimenziji" sheetId="2" r:id="rId1"/>
     <sheet name="3 dimenzije" sheetId="1" r:id="rId2"/>
     <sheet name="4 dimenzije" sheetId="3" r:id="rId3"/>
     <sheet name="5 dimenzij" sheetId="4" r:id="rId4"/>
-    <sheet name="Grafi" sheetId="5" r:id="rId5"/>
+    <sheet name="Grafi 1" sheetId="5" r:id="rId5"/>
+    <sheet name="krogla vs kocka" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="29">
   <si>
     <t>1. pareto fornta</t>
   </si>
@@ -93,12 +94,45 @@
   <si>
     <t>5 dimenzij krogla</t>
   </si>
+  <si>
+    <t>Primerjava krogle in kocke</t>
+  </si>
+  <si>
+    <t>1. Pareto fronta</t>
+  </si>
+  <si>
+    <t>2. Pareto fronta</t>
+  </si>
+  <si>
+    <t>3. Pareto fronta</t>
+  </si>
+  <si>
+    <t>4. Pareto fronta</t>
+  </si>
+  <si>
+    <t>5. Pareto Fronta</t>
+  </si>
+  <si>
+    <t>Za vsako 20 poskusov po 500 točk 5 dimenzij</t>
+  </si>
+  <si>
+    <t>KROGLA</t>
+  </si>
+  <si>
+    <t>št. Poskusa</t>
+  </si>
+  <si>
+    <t>Povprečno</t>
+  </si>
+  <si>
+    <t>KOCKA</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -122,6 +156,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -137,7 +179,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -145,11 +187,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -161,6 +289,33 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2611,6 +2766,401 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-GB"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Povprečno</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-GB" baseline="0"/>
+              <a:t> število točk v prvih petih Pareto forntah</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-SI"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'krogla vs kocka'!$C$30</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KROGLA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'krogla vs kocka'!$D$30:$H$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>90.35</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>147.30000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>131.75</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>80.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3A10-484A-80ED-C43FD13CE886}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'krogla vs kocka'!$C$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>KOCKA</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'krogla vs kocka'!$D$55:$H$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>118.75</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>158.19999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>123.25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>68.8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26.05</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3A10-484A-80ED-C43FD13CE886}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="2120282560"/>
+        <c:axId val="2122705600"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="2120282560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-SI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2122705600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2122705600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-SI"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2120282560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-SI"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-SI"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2811,6 +3361,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
@@ -4876,6 +5466,522 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -5581,6 +6687,47 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1092200</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>69850</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A16E84D-6A07-8240-BB04-FBCB725D9A83}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5888,7 +7035,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3030A96B-6BCE-A34B-9F15-40CDBF632279}">
   <dimension ref="B2:I45"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="I29" sqref="I29"/>
     </sheetView>
   </sheetViews>
@@ -10148,7 +11295,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8211CCAC-B6B2-C840-8888-235AA45152A3}">
   <dimension ref="B2:O33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
@@ -10670,4 +11817,1118 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9DC9115-B667-9F4D-A319-7B191B68D1E6}">
+  <dimension ref="B2:I55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="M66" sqref="M66"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.1640625" customWidth="1"/>
+    <col min="4" max="8" width="13.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:9" ht="16" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="9"/>
+    </row>
+    <row r="4" spans="2:9" ht="16" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="12"/>
+    </row>
+    <row r="5" spans="2:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="14"/>
+      <c r="D5" s="14"/>
+      <c r="E5" s="14"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>75</v>
+      </c>
+      <c r="E10">
+        <v>119</v>
+      </c>
+      <c r="F10">
+        <v>166</v>
+      </c>
+      <c r="G10">
+        <v>86</v>
+      </c>
+      <c r="H10">
+        <v>31</v>
+      </c>
+      <c r="I10">
+        <f>SUM(D10:H10)</f>
+        <v>477</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>2</v>
+      </c>
+      <c r="D11">
+        <v>92</v>
+      </c>
+      <c r="E11">
+        <v>172</v>
+      </c>
+      <c r="F11">
+        <v>146</v>
+      </c>
+      <c r="G11">
+        <v>59</v>
+      </c>
+      <c r="H11">
+        <v>12</v>
+      </c>
+      <c r="I11">
+        <f t="shared" ref="I11:I30" si="0">SUM(D11:H11)</f>
+        <v>481</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>3</v>
+      </c>
+      <c r="D12">
+        <v>76</v>
+      </c>
+      <c r="E12">
+        <v>120</v>
+      </c>
+      <c r="F12">
+        <v>112</v>
+      </c>
+      <c r="G12">
+        <v>101</v>
+      </c>
+      <c r="H12">
+        <v>62</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="0"/>
+        <v>471</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>4</v>
+      </c>
+      <c r="D13">
+        <v>94</v>
+      </c>
+      <c r="E13">
+        <v>128</v>
+      </c>
+      <c r="F13">
+        <v>137</v>
+      </c>
+      <c r="G13">
+        <v>86</v>
+      </c>
+      <c r="H13">
+        <v>33</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="0"/>
+        <v>478</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>5</v>
+      </c>
+      <c r="D14">
+        <v>100</v>
+      </c>
+      <c r="E14">
+        <v>128</v>
+      </c>
+      <c r="F14">
+        <v>138</v>
+      </c>
+      <c r="G14">
+        <v>90</v>
+      </c>
+      <c r="H14">
+        <v>28</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="0"/>
+        <v>484</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>6</v>
+      </c>
+      <c r="D15">
+        <v>103</v>
+      </c>
+      <c r="E15">
+        <v>174</v>
+      </c>
+      <c r="F15">
+        <v>110</v>
+      </c>
+      <c r="G15">
+        <v>67</v>
+      </c>
+      <c r="H15">
+        <v>20</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="0"/>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>95</v>
+      </c>
+      <c r="E16">
+        <v>145</v>
+      </c>
+      <c r="F16">
+        <v>141</v>
+      </c>
+      <c r="G16">
+        <v>81</v>
+      </c>
+      <c r="H16">
+        <v>18</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>88</v>
+      </c>
+      <c r="E17">
+        <v>191</v>
+      </c>
+      <c r="F17">
+        <v>142</v>
+      </c>
+      <c r="G17">
+        <v>49</v>
+      </c>
+      <c r="H17">
+        <v>16</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="0"/>
+        <v>486</v>
+      </c>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>93</v>
+      </c>
+      <c r="E18">
+        <v>158</v>
+      </c>
+      <c r="F18">
+        <v>156</v>
+      </c>
+      <c r="G18">
+        <v>66</v>
+      </c>
+      <c r="H18">
+        <v>18</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="0"/>
+        <v>491</v>
+      </c>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <v>95</v>
+      </c>
+      <c r="E19">
+        <v>171</v>
+      </c>
+      <c r="F19">
+        <v>113</v>
+      </c>
+      <c r="G19">
+        <v>75</v>
+      </c>
+      <c r="H19">
+        <v>24</v>
+      </c>
+      <c r="I19">
+        <f t="shared" si="0"/>
+        <v>478</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>11</v>
+      </c>
+      <c r="D20">
+        <v>101</v>
+      </c>
+      <c r="E20">
+        <v>144</v>
+      </c>
+      <c r="F20">
+        <v>98</v>
+      </c>
+      <c r="G20">
+        <v>92</v>
+      </c>
+      <c r="H20">
+        <v>34</v>
+      </c>
+      <c r="I20">
+        <f t="shared" si="0"/>
+        <v>469</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>12</v>
+      </c>
+      <c r="D21">
+        <v>96</v>
+      </c>
+      <c r="E21">
+        <v>149</v>
+      </c>
+      <c r="F21">
+        <v>120</v>
+      </c>
+      <c r="G21">
+        <v>88</v>
+      </c>
+      <c r="H21">
+        <v>30</v>
+      </c>
+      <c r="I21">
+        <f t="shared" si="0"/>
+        <v>483</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>13</v>
+      </c>
+      <c r="D22">
+        <v>70</v>
+      </c>
+      <c r="E22">
+        <v>159</v>
+      </c>
+      <c r="F22">
+        <v>135</v>
+      </c>
+      <c r="G22">
+        <v>97</v>
+      </c>
+      <c r="H22">
+        <v>20</v>
+      </c>
+      <c r="I22">
+        <f t="shared" si="0"/>
+        <v>481</v>
+      </c>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>14</v>
+      </c>
+      <c r="D23">
+        <v>96</v>
+      </c>
+      <c r="E23">
+        <v>137</v>
+      </c>
+      <c r="F23">
+        <v>134</v>
+      </c>
+      <c r="G23">
+        <v>86</v>
+      </c>
+      <c r="H23">
+        <v>26</v>
+      </c>
+      <c r="I23">
+        <f t="shared" si="0"/>
+        <v>479</v>
+      </c>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>15</v>
+      </c>
+      <c r="D24">
+        <v>88</v>
+      </c>
+      <c r="E24">
+        <v>112</v>
+      </c>
+      <c r="F24">
+        <v>126</v>
+      </c>
+      <c r="G24">
+        <v>111</v>
+      </c>
+      <c r="H24">
+        <v>41</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="0"/>
+        <v>478</v>
+      </c>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>16</v>
+      </c>
+      <c r="D25">
+        <v>76</v>
+      </c>
+      <c r="E25">
+        <v>122</v>
+      </c>
+      <c r="F25">
+        <v>109</v>
+      </c>
+      <c r="G25">
+        <v>82</v>
+      </c>
+      <c r="H25">
+        <v>72</v>
+      </c>
+      <c r="I25">
+        <f t="shared" si="0"/>
+        <v>461</v>
+      </c>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>17</v>
+      </c>
+      <c r="D26">
+        <v>118</v>
+      </c>
+      <c r="E26">
+        <v>176</v>
+      </c>
+      <c r="F26">
+        <v>127</v>
+      </c>
+      <c r="G26">
+        <v>58</v>
+      </c>
+      <c r="H26">
+        <v>16</v>
+      </c>
+      <c r="I26">
+        <f t="shared" si="0"/>
+        <v>495</v>
+      </c>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>18</v>
+      </c>
+      <c r="D27">
+        <v>99</v>
+      </c>
+      <c r="E27">
+        <v>134</v>
+      </c>
+      <c r="F27">
+        <v>141</v>
+      </c>
+      <c r="G27">
+        <v>75</v>
+      </c>
+      <c r="H27">
+        <v>30</v>
+      </c>
+      <c r="I27">
+        <f t="shared" si="0"/>
+        <v>479</v>
+      </c>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>19</v>
+      </c>
+      <c r="D28">
+        <v>92</v>
+      </c>
+      <c r="E28">
+        <v>159</v>
+      </c>
+      <c r="F28">
+        <v>138</v>
+      </c>
+      <c r="G28">
+        <v>66</v>
+      </c>
+      <c r="H28">
+        <v>24</v>
+      </c>
+      <c r="I28">
+        <f t="shared" si="0"/>
+        <v>479</v>
+      </c>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>20</v>
+      </c>
+      <c r="D29">
+        <v>60</v>
+      </c>
+      <c r="E29">
+        <v>148</v>
+      </c>
+      <c r="F29">
+        <v>146</v>
+      </c>
+      <c r="G29">
+        <v>95</v>
+      </c>
+      <c r="H29">
+        <v>25</v>
+      </c>
+      <c r="I29">
+        <f t="shared" si="0"/>
+        <v>474</v>
+      </c>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D30">
+        <f>AVERAGE(D10:D29)</f>
+        <v>90.35</v>
+      </c>
+      <c r="E30">
+        <f t="shared" ref="E30:H30" si="1">AVERAGE(E10:E29)</f>
+        <v>147.30000000000001</v>
+      </c>
+      <c r="F30">
+        <f t="shared" si="1"/>
+        <v>131.75</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>80.5</v>
+      </c>
+      <c r="H30">
+        <f t="shared" si="1"/>
+        <v>29</v>
+      </c>
+      <c r="I30">
+        <f t="shared" si="0"/>
+        <v>478.9</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C34" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C35">
+        <v>1</v>
+      </c>
+      <c r="D35">
+        <v>111</v>
+      </c>
+      <c r="E35">
+        <v>172</v>
+      </c>
+      <c r="F35">
+        <v>129</v>
+      </c>
+      <c r="G35">
+        <v>67</v>
+      </c>
+      <c r="H35">
+        <v>20</v>
+      </c>
+      <c r="I35">
+        <f>SUM(D35:H35)</f>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>128</v>
+      </c>
+      <c r="E36">
+        <v>155</v>
+      </c>
+      <c r="F36">
+        <v>116</v>
+      </c>
+      <c r="G36">
+        <v>77</v>
+      </c>
+      <c r="H36">
+        <v>23</v>
+      </c>
+      <c r="I36">
+        <f t="shared" ref="I36:I55" si="2">SUM(D36:H36)</f>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C37">
+        <v>3</v>
+      </c>
+      <c r="D37">
+        <v>104</v>
+      </c>
+      <c r="E37">
+        <v>137</v>
+      </c>
+      <c r="F37">
+        <v>129</v>
+      </c>
+      <c r="G37">
+        <v>79</v>
+      </c>
+      <c r="H37">
+        <v>43</v>
+      </c>
+      <c r="I37">
+        <f t="shared" si="2"/>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="38" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C38">
+        <v>4</v>
+      </c>
+      <c r="D38">
+        <v>115</v>
+      </c>
+      <c r="E38">
+        <v>117</v>
+      </c>
+      <c r="F38">
+        <v>130</v>
+      </c>
+      <c r="G38">
+        <v>79</v>
+      </c>
+      <c r="H38">
+        <v>51</v>
+      </c>
+      <c r="I38">
+        <f t="shared" si="2"/>
+        <v>492</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C39">
+        <v>5</v>
+      </c>
+      <c r="D39">
+        <v>139</v>
+      </c>
+      <c r="E39">
+        <v>153</v>
+      </c>
+      <c r="F39">
+        <v>124</v>
+      </c>
+      <c r="G39">
+        <v>58</v>
+      </c>
+      <c r="H39">
+        <v>21</v>
+      </c>
+      <c r="I39">
+        <f t="shared" si="2"/>
+        <v>495</v>
+      </c>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C40">
+        <v>6</v>
+      </c>
+      <c r="D40">
+        <v>98</v>
+      </c>
+      <c r="E40">
+        <v>167</v>
+      </c>
+      <c r="F40">
+        <v>122</v>
+      </c>
+      <c r="G40">
+        <v>79</v>
+      </c>
+      <c r="H40">
+        <v>33</v>
+      </c>
+      <c r="I40">
+        <f t="shared" si="2"/>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C41">
+        <v>7</v>
+      </c>
+      <c r="D41">
+        <v>119</v>
+      </c>
+      <c r="E41">
+        <v>160</v>
+      </c>
+      <c r="F41">
+        <v>128</v>
+      </c>
+      <c r="G41">
+        <v>64</v>
+      </c>
+      <c r="H41">
+        <v>22</v>
+      </c>
+      <c r="I41">
+        <f t="shared" si="2"/>
+        <v>493</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C42">
+        <v>8</v>
+      </c>
+      <c r="D42">
+        <v>112</v>
+      </c>
+      <c r="E42">
+        <v>185</v>
+      </c>
+      <c r="F42">
+        <v>118</v>
+      </c>
+      <c r="G42">
+        <v>64</v>
+      </c>
+      <c r="H42">
+        <v>17</v>
+      </c>
+      <c r="I42">
+        <f t="shared" si="2"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C43">
+        <v>9</v>
+      </c>
+      <c r="D43">
+        <v>139</v>
+      </c>
+      <c r="E43">
+        <v>147</v>
+      </c>
+      <c r="F43">
+        <v>125</v>
+      </c>
+      <c r="G43">
+        <v>52</v>
+      </c>
+      <c r="H43">
+        <v>23</v>
+      </c>
+      <c r="I43">
+        <f t="shared" si="2"/>
+        <v>486</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C44">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>125</v>
+      </c>
+      <c r="E44">
+        <v>159</v>
+      </c>
+      <c r="F44">
+        <v>128</v>
+      </c>
+      <c r="G44">
+        <v>69</v>
+      </c>
+      <c r="H44">
+        <v>14</v>
+      </c>
+      <c r="I44">
+        <f t="shared" si="2"/>
+        <v>495</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C45">
+        <v>11</v>
+      </c>
+      <c r="D45">
+        <v>146</v>
+      </c>
+      <c r="E45">
+        <v>171</v>
+      </c>
+      <c r="F45">
+        <v>113</v>
+      </c>
+      <c r="G45">
+        <v>55</v>
+      </c>
+      <c r="H45">
+        <v>13</v>
+      </c>
+      <c r="I45">
+        <f t="shared" si="2"/>
+        <v>498</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C46">
+        <v>12</v>
+      </c>
+      <c r="D46">
+        <v>123</v>
+      </c>
+      <c r="E46">
+        <v>162</v>
+      </c>
+      <c r="F46">
+        <v>129</v>
+      </c>
+      <c r="G46">
+        <v>74</v>
+      </c>
+      <c r="H46">
+        <v>12</v>
+      </c>
+      <c r="I46">
+        <f t="shared" si="2"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C47">
+        <v>13</v>
+      </c>
+      <c r="D47">
+        <v>99</v>
+      </c>
+      <c r="E47">
+        <v>164</v>
+      </c>
+      <c r="F47">
+        <v>101</v>
+      </c>
+      <c r="G47">
+        <v>73</v>
+      </c>
+      <c r="H47">
+        <v>46</v>
+      </c>
+      <c r="I47">
+        <f t="shared" si="2"/>
+        <v>483</v>
+      </c>
+    </row>
+    <row r="48" spans="3:9" x14ac:dyDescent="0.2">
+      <c r="C48">
+        <v>14</v>
+      </c>
+      <c r="D48">
+        <v>111</v>
+      </c>
+      <c r="E48">
+        <v>146</v>
+      </c>
+      <c r="F48">
+        <v>132</v>
+      </c>
+      <c r="G48">
+        <v>69</v>
+      </c>
+      <c r="H48">
+        <v>36</v>
+      </c>
+      <c r="I48">
+        <f t="shared" si="2"/>
+        <v>494</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C49">
+        <v>15</v>
+      </c>
+      <c r="D49">
+        <v>119</v>
+      </c>
+      <c r="E49">
+        <v>179</v>
+      </c>
+      <c r="F49">
+        <v>118</v>
+      </c>
+      <c r="G49">
+        <v>67</v>
+      </c>
+      <c r="H49">
+        <v>15</v>
+      </c>
+      <c r="I49">
+        <f t="shared" si="2"/>
+        <v>498</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C50">
+        <v>16</v>
+      </c>
+      <c r="D50">
+        <v>134</v>
+      </c>
+      <c r="E50">
+        <v>162</v>
+      </c>
+      <c r="F50">
+        <v>111</v>
+      </c>
+      <c r="G50">
+        <v>62</v>
+      </c>
+      <c r="H50">
+        <v>29</v>
+      </c>
+      <c r="I50">
+        <f t="shared" si="2"/>
+        <v>498</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C51">
+        <v>17</v>
+      </c>
+      <c r="D51">
+        <v>113</v>
+      </c>
+      <c r="E51">
+        <v>159</v>
+      </c>
+      <c r="F51">
+        <v>122</v>
+      </c>
+      <c r="G51">
+        <v>81</v>
+      </c>
+      <c r="H51">
+        <v>23</v>
+      </c>
+      <c r="I51">
+        <f t="shared" si="2"/>
+        <v>498</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C52">
+        <v>18</v>
+      </c>
+      <c r="D52">
+        <v>138</v>
+      </c>
+      <c r="E52">
+        <v>145</v>
+      </c>
+      <c r="F52">
+        <v>123</v>
+      </c>
+      <c r="G52">
+        <v>67</v>
+      </c>
+      <c r="H52">
+        <v>23</v>
+      </c>
+      <c r="I52">
+        <f t="shared" si="2"/>
+        <v>496</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C53">
+        <v>19</v>
+      </c>
+      <c r="D53">
+        <v>94</v>
+      </c>
+      <c r="E53">
+        <v>187</v>
+      </c>
+      <c r="F53">
+        <v>138</v>
+      </c>
+      <c r="G53">
+        <v>60</v>
+      </c>
+      <c r="H53">
+        <v>20</v>
+      </c>
+      <c r="I53">
+        <f t="shared" si="2"/>
+        <v>499</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="C54">
+        <v>20</v>
+      </c>
+      <c r="D54">
+        <v>108</v>
+      </c>
+      <c r="E54">
+        <v>137</v>
+      </c>
+      <c r="F54">
+        <v>129</v>
+      </c>
+      <c r="G54">
+        <v>80</v>
+      </c>
+      <c r="H54">
+        <v>37</v>
+      </c>
+      <c r="I54">
+        <f t="shared" si="2"/>
+        <v>491</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D55">
+        <f>AVERAGE(D35:D54)</f>
+        <v>118.75</v>
+      </c>
+      <c r="E55">
+        <f t="shared" ref="E55" si="3">AVERAGE(E35:E54)</f>
+        <v>158.19999999999999</v>
+      </c>
+      <c r="F55">
+        <f t="shared" ref="F55" si="4">AVERAGE(F35:F54)</f>
+        <v>123.25</v>
+      </c>
+      <c r="G55">
+        <f t="shared" ref="G55" si="5">AVERAGE(G35:G54)</f>
+        <v>68.8</v>
+      </c>
+      <c r="H55">
+        <f t="shared" ref="H55" si="6">AVERAGE(H35:H54)</f>
+        <v>26.05</v>
+      </c>
+      <c r="I55">
+        <f t="shared" si="2"/>
+        <v>495.05</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B3:F4"/>
+    <mergeCell ref="B5:F5"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>